<commit_message>
added devise, updated devise sign up, added select_tag, added sort for index page
</commit_message>
<xml_diff>
--- a/capstone_schema.xlsx
+++ b/capstone_schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6400" yWindow="-23540" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="-8040" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
   <si>
     <t>User</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>has_many :attended_events through user_events</t>
+  </si>
+  <si>
+    <t>profile_url</t>
   </si>
 </sst>
 </file>
@@ -492,9 +495,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -510,6 +510,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -810,7 +813,7 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,7 +859,7 @@
         <v>20</v>
       </c>
       <c r="F2" s="5"/>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="35" t="s">
         <v>29</v>
       </c>
     </row>
@@ -873,7 +876,7 @@
         <v>23</v>
       </c>
       <c r="F3" s="5"/>
-      <c r="N3" s="24"/>
+      <c r="N3" s="35"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
@@ -886,7 +889,7 @@
         <v>38</v>
       </c>
       <c r="F4" s="16"/>
-      <c r="N4" s="24"/>
+      <c r="N4" s="35"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -897,7 +900,7 @@
       <c r="D5" s="16"/>
       <c r="E5" s="15"/>
       <c r="F5" s="16"/>
-      <c r="N5" s="24"/>
+      <c r="N5" s="35"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -908,7 +911,7 @@
       <c r="D6" s="16"/>
       <c r="E6" s="15"/>
       <c r="F6" s="16"/>
-      <c r="N6" s="24"/>
+      <c r="N6" s="35"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
@@ -919,7 +922,7 @@
       <c r="D7" s="16"/>
       <c r="E7" s="15"/>
       <c r="F7" s="16"/>
-      <c r="N7" s="24"/>
+      <c r="N7" s="35"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
@@ -930,7 +933,7 @@
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
       <c r="F8" s="16"/>
-      <c r="N8" s="24"/>
+      <c r="N8" s="35"/>
     </row>
     <row r="9" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -939,7 +942,7 @@
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
-      <c r="N9" s="24"/>
+      <c r="N9" s="35"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
@@ -1007,7 +1010,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>4</v>
@@ -1049,7 +1052,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="31" t="s">
         <v>27</v>
       </c>
       <c r="F18" s="5"/>
@@ -1063,13 +1066,13 @@
         <v>27</v>
       </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="31" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="5"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="29"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -1080,9 +1083,9 @@
       <c r="D20" s="5"/>
       <c r="E20" s="15"/>
       <c r="F20" s="16"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
@@ -1093,9 +1096,9 @@
       <c r="D21" s="16"/>
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
@@ -1104,13 +1107,13 @@
       <c r="B22" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="32" t="s">
         <v>36</v>
       </c>
       <c r="F22" s="8" t="s">
@@ -1118,19 +1121,19 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="33" t="s">
         <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="31" t="s">
         <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -1138,13 +1141,13 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="33" t="s">
         <v>16</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="26"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="5"/>
       <c r="E24" s="4" t="s">
         <v>42</v>
@@ -1156,7 +1159,7 @@
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="26"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="5"/>
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
@@ -1165,10 +1168,10 @@
       <c r="A26" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="26"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="5"/>
       <c r="E26" s="15"/>
       <c r="F26" s="16"/>
@@ -1177,10 +1180,10 @@
       <c r="A27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="27"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="16"/>
       <c r="E27" s="6"/>
       <c r="F27" s="7"/>
@@ -1192,7 +1195,7 @@
       <c r="B28" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="28"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>